<commit_message>
code-base organization wave 1
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pengu\AppData\Roaming\Factorio\mods\rufmorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D79DFFE-5A95-45A2-8052-D79402EE0CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F92651D-5DB9-474C-8117-F3B203D9E17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{27854B9F-89A4-4BA3-8F55-AED8505BFCBF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{27854B9F-89A4-4BA3-8F55-AED8505BFCBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="159">
   <si>
     <t>Recipes</t>
   </si>
@@ -469,6 +469,51 @@
   </si>
   <si>
     <t>Electric Lab</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Fish Farm</t>
+  </si>
+  <si>
+    <t>4x Raw Fish, 100x Muddy Water</t>
+  </si>
+  <si>
+    <t>Fish Eggs</t>
+  </si>
+  <si>
+    <t>2x Fish</t>
+  </si>
+  <si>
+    <t>Render Fish</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>Butchering Machine</t>
+  </si>
+  <si>
+    <t>1x Fish</t>
+  </si>
+  <si>
+    <t>2x Fish Meat, 1x Fish Brain, 1x Fish Intestines, 1x Fish Heart, 4x Fish Fins, 2x Fish Eyes, 1x Wet Fish Bladder</t>
+  </si>
+  <si>
+    <t>5x Wet Fish Bladder</t>
+  </si>
+  <si>
+    <t>50x Fish Oil</t>
+  </si>
+  <si>
+    <t>100x Water (Fish Egg Modules effect crafting speed)</t>
+  </si>
+  <si>
+    <t>2x Fish Eggs, 2x Spent Fish</t>
   </si>
 </sst>
 </file>
@@ -822,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -925,6 +970,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -935,6 +998,39 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -943,86 +1039,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B220E3-4B6F-4A08-9714-1CD525B71314}">
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:W148"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33:S33"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38:S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,27 +1418,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="60"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="69"/>
       <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1401,33 +1447,33 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="58" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="68" t="s">
+      <c r="F2" s="68"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="62" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="63"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="49"/>
       <c r="V2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1436,33 +1482,33 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="61" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="62"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="66" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="64" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="65"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="60"/>
       <c r="V3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1471,33 +1517,33 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="44" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="50" t="s">
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="51" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="52"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="55"/>
       <c r="V4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1506,33 +1552,33 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="44" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="50" t="s">
+      <c r="F5" s="51"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="51" t="s">
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="52"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="55"/>
       <c r="V5" s="1" t="s">
         <v>48</v>
       </c>
@@ -1541,33 +1587,33 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="44" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="50" t="s">
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="51" t="s">
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="51"/>
-      <c r="S6" s="52"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="55"/>
       <c r="V6" s="1" t="s">
         <v>50</v>
       </c>
@@ -1576,33 +1622,33 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="50" t="s">
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="51" t="s">
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="51"/>
-      <c r="S7" s="52"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="55"/>
       <c r="V7" s="1" t="s">
         <v>57</v>
       </c>
@@ -1611,33 +1657,33 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="44" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="50" t="s">
+      <c r="F8" s="51"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="51" t="s">
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="52"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="55"/>
       <c r="V8" s="1" t="s">
         <v>66</v>
       </c>
@@ -1646,33 +1692,33 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="44" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="50" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="51" t="s">
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="52"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="55"/>
       <c r="V9" s="1" t="s">
         <v>72</v>
       </c>
@@ -1681,33 +1727,33 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="44" t="s">
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="50" t="s">
+      <c r="F10" s="51"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="51" t="s">
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="52"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="55"/>
       <c r="V10" s="1" t="s">
         <v>83</v>
       </c>
@@ -1716,33 +1762,33 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="44" t="s">
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="50" t="s">
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="51" t="s">
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="52"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="55"/>
       <c r="V11" s="1" t="s">
         <v>88</v>
       </c>
@@ -1751,33 +1797,33 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="44" t="s">
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="50" t="s">
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="51" t="s">
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="52"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="55"/>
       <c r="V12" s="1" t="s">
         <v>100</v>
       </c>
@@ -1786,33 +1832,33 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="44" t="s">
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="50" t="s">
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="51" t="s">
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="52"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="55"/>
       <c r="V13" s="1" t="s">
         <v>102</v>
       </c>
@@ -1821,33 +1867,33 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="44" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="50" t="s">
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="51" t="s">
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="52"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="55"/>
       <c r="V14" s="1" t="s">
         <v>106</v>
       </c>
@@ -1856,658 +1902,982 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="44" t="s">
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="45"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="50" t="s">
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="51" t="s">
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="52"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="55"/>
+      <c r="V15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="44" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="50" t="s">
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="51" t="s">
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="52"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="55"/>
+      <c r="V16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="44" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="47" t="s">
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="47" t="s">
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
-      <c r="S17" s="49"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="66"/>
     </row>
     <row r="18" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="44" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47" t="s">
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="47" t="s">
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="49"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="66"/>
     </row>
     <row r="19" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="44" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47" t="s">
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="47" t="s">
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="49"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="65"/>
+      <c r="S19" s="66"/>
     </row>
     <row r="20" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="44" t="s">
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="47" t="s">
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="47" t="s">
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="49"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="66"/>
     </row>
     <row r="21" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="44" t="s">
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47" t="s">
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="47" t="s">
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="49"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="65"/>
+      <c r="S21" s="66"/>
     </row>
     <row r="22" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="44" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="45"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="50" t="s">
+      <c r="F22" s="51"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="51" t="s">
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="52"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="55"/>
     </row>
     <row r="23" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="44" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="50" t="s">
+      <c r="F23" s="51"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="51" t="s">
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="52"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="55"/>
     </row>
     <row r="24" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="44" t="s">
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="50" t="s">
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="51" t="s">
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="52"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="55"/>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="44" t="s">
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="50" t="s">
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="51" t="s">
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="52"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="55"/>
     </row>
     <row r="26" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="44" t="s">
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="45"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="50" t="s">
+      <c r="F26" s="51"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="51" t="s">
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="52"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="55"/>
     </row>
     <row r="27" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="44" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="47" t="s">
+      <c r="F27" s="51"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="47" t="s">
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="48"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="49"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="66"/>
     </row>
     <row r="28" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="44" t="s">
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="50" t="s">
+      <c r="F28" s="51"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="51" t="s">
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="52"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="55"/>
     </row>
     <row r="29" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="44" t="s">
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="50" t="s">
+      <c r="F29" s="51"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="51" t="s">
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="52"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="55"/>
     </row>
     <row r="30" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="44" t="s">
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="50" t="s">
+      <c r="F30" s="51"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="51" t="s">
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="52"/>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="55"/>
     </row>
     <row r="31" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="44" t="s">
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="47" t="s">
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="47" t="s">
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-      <c r="S31" s="49"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="65"/>
+      <c r="S31" s="66"/>
     </row>
     <row r="32" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="44" t="s">
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="F32" s="45"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="47" t="s">
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="47" t="s">
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="O32" s="48"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
-      <c r="R32" s="48"/>
-      <c r="S32" s="49"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="65"/>
+      <c r="S32" s="66"/>
     </row>
     <row r="33" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="44" t="s">
+      <c r="B33" s="51"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="50" t="s">
+      <c r="F33" s="51"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="51" t="s">
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="51"/>
-      <c r="S33" s="52"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="55"/>
     </row>
     <row r="34" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="44" t="s">
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="45"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="50" t="s">
+      <c r="F34" s="51"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="51" t="s">
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="52"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="54"/>
+      <c r="S34" s="55"/>
     </row>
     <row r="35" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="44" t="s">
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="50" t="s">
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="51" t="s">
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="54"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="52"/>
+      <c r="O35" s="54"/>
+      <c r="P35" s="54"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="55"/>
     </row>
     <row r="36" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="51"/>
-      <c r="O36" s="51"/>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="51"/>
-      <c r="S36" s="52"/>
+      <c r="A36" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36" s="51"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" s="54"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="54"/>
+      <c r="S36" s="55"/>
     </row>
     <row r="37" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="57"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="57"/>
-    </row>
+      <c r="A37" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="57"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
+      <c r="Q37" s="62"/>
+      <c r="R37" s="62"/>
+      <c r="S37" s="63"/>
+    </row>
+    <row r="38" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="O38" s="76"/>
+      <c r="P38" s="76"/>
+      <c r="Q38" s="76"/>
+      <c r="R38" s="76"/>
+      <c r="S38" s="76"/>
+    </row>
+    <row r="39" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+    </row>
+    <row r="40" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="145">
+  <mergeCells count="153">
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:M39"/>
+    <mergeCell ref="N39:S39"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="N32:S32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="N20:S20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="N21:S21"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="N18:S18"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="N17:S17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="N19:S19"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="N37:S37"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="N29:S29"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N34:S34"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N36:S36"/>
+    <mergeCell ref="N22:S22"/>
+    <mergeCell ref="N23:S23"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="N3:S3"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="N6:S6"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="N8:S8"/>
+    <mergeCell ref="N9:S9"/>
+    <mergeCell ref="N10:S10"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N25:S25"/>
+    <mergeCell ref="N26:S26"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N11:S11"/>
+    <mergeCell ref="N12:S12"/>
+    <mergeCell ref="N13:S13"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="N15:S15"/>
+    <mergeCell ref="N16:S16"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="H2:M2"/>
     <mergeCell ref="N2:S2"/>
@@ -2532,127 +2902,6 @@
     <mergeCell ref="H12:M12"/>
     <mergeCell ref="H13:M13"/>
     <mergeCell ref="H14:M14"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="N3:S3"/>
-    <mergeCell ref="N4:S4"/>
-    <mergeCell ref="N5:S5"/>
-    <mergeCell ref="N6:S6"/>
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="N8:S8"/>
-    <mergeCell ref="N9:S9"/>
-    <mergeCell ref="N10:S10"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N25:S25"/>
-    <mergeCell ref="N26:S26"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N11:S11"/>
-    <mergeCell ref="N12:S12"/>
-    <mergeCell ref="N13:S13"/>
-    <mergeCell ref="N14:S14"/>
-    <mergeCell ref="N15:S15"/>
-    <mergeCell ref="N16:S16"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N37:S37"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="N29:S29"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N34:S34"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N36:S36"/>
-    <mergeCell ref="N22:S22"/>
-    <mergeCell ref="N23:S23"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="N18:S18"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="N17:S17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="N19:S19"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="N32:S32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="N20:S20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="N21:S21"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="A27:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2663,7 +2912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E4471D-F598-4019-87E9-33CC87DA5334}">
   <dimension ref="B14:AC50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
@@ -2688,9 +2937,9 @@
       <c r="H15" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="75"/>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
@@ -2724,22 +2973,15 @@
         <v>139</v>
       </c>
       <c r="G21" s="72"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="F22" s="12"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="77"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="F23" s="9"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="77"/>
+      <c r="J23" s="12"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="F24" s="71" t="s">
@@ -2990,7 +3232,7 @@
       <c r="E36" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="F36" s="74"/>
+      <c r="F36" s="73"/>
       <c r="G36" s="5"/>
       <c r="H36" s="71" t="s">
         <v>130</v>
@@ -3438,32 +3680,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>